<commit_message>
Innovations doc added and test plan added too
</commit_message>
<xml_diff>
--- a/Test Plan.xlsx
+++ b/Test Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Desktop\G00347352 - Advanced DataCentric Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C143663-D70C-45AE-9E7D-A70AAF64D407}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA6365E-34EB-4EF9-AF56-96A3F1FABE52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27015" yWindow="3375" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="114">
   <si>
     <t>Project Name</t>
   </si>
@@ -216,9 +216,6 @@
     <t>TC.001</t>
   </si>
   <si>
-    <t>GUI</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
@@ -255,141 +252,7 @@
     <t>Final run through of the entire application</t>
   </si>
   <si>
-    <t>Icons Displaying</t>
-  </si>
-  <si>
-    <t>1. Launch Application</t>
-  </si>
-  <si>
-    <t>Checks if the app logo is displayed on the splash screen</t>
-  </si>
-  <si>
-    <t>Logo is displayed on the splash screen</t>
-  </si>
-  <si>
-    <t>Logo was displayed when I launched the application</t>
-  </si>
-  <si>
-    <t>Download data</t>
-  </si>
-  <si>
     <t>Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Launch Application
-</t>
-  </si>
-  <si>
-    <t>checks if Game Stats are downloaded in the Background as the app is loading</t>
-  </si>
-  <si>
-    <t>Games stats are downloaded</t>
-  </si>
-  <si>
-    <t>Game stats are downloaded and displayed in the console window for debugging and in the Game Stats page</t>
-  </si>
-  <si>
-    <t>View Game Stats</t>
-  </si>
-  <si>
-    <t>1. Launch Application
-2. Click View Game Statistics</t>
-  </si>
-  <si>
-    <t>Checks if you can see game history and statistics</t>
-  </si>
-  <si>
-    <t>Game Stats are displayed in a list view</t>
-  </si>
-  <si>
-    <t>Game stats are there to view</t>
-  </si>
-  <si>
-    <t>Refresh Game Stats</t>
-  </si>
-  <si>
-    <t>1. Launch Application
-2. Create new game
-3.Enter Details
-4.Start New Game
-5. Finish Game
-6. Return to Game Statistic Page and click refresh</t>
-  </si>
-  <si>
-    <t>Checks if you can see new game stats after completing a game</t>
-  </si>
-  <si>
-    <t>New Game Stats are displayed</t>
-  </si>
-  <si>
-    <t>Checkout Data
- Downloaded</t>
-  </si>
-  <si>
-    <t>1. Launch Application
-2. Click Create New Game</t>
-  </si>
-  <si>
-    <t>Data Downloaded and outputed to console</t>
-  </si>
-  <si>
-    <t>Checkout Data is downloaded and outputted to console for debugging</t>
-  </si>
-  <si>
-    <t>User Input</t>
-  </si>
-  <si>
-    <t>1. Launch Application
-2. Click Create New Game
-3. Click Start new Game with missing values</t>
-  </si>
-  <si>
-    <t>Checks if Checkout Data is downloaded from MONGO</t>
-  </si>
-  <si>
-    <t>Checks if alert is displayed if 1 or more values is missing</t>
-  </si>
-  <si>
-    <t>Alert pops up</t>
-  </si>
-  <si>
-    <t>Alert did display alerting the user that all values must be filled in</t>
-  </si>
-  <si>
-    <t>Player Win</t>
-  </si>
-  <si>
-    <t>1. Launch Application
-2. Click Create New Game
-3. Enter all values
-4. Make one player win the sets</t>
-  </si>
-  <si>
-    <t>Checks if a player can win the match</t>
-  </si>
-  <si>
-    <t>Alert pops up saying who won</t>
-  </si>
-  <si>
-    <t>Alert did display alerting the user that the match is over and who won</t>
-  </si>
-  <si>
-    <t>Backup File</t>
-  </si>
-  <si>
-    <t>1. Launch Application
-2. Click Create New Game
-3. Enter all values
-5.Click Start new game</t>
-  </si>
-  <si>
-    <t>Checks if checkout data is retrieved from a backup file if there is no internet connection</t>
-  </si>
-  <si>
-    <t>Data should be seen in the console window</t>
-  </si>
-  <si>
-    <t>Data is seen in the console window</t>
   </si>
   <si>
     <t>Test Advanced Data Centric Project</t>
@@ -397,6 +260,187 @@
   <si>
     <t xml:space="preserve">
 Windows 10</t>
+  </si>
+  <si>
+    <t>Page Navigation</t>
+  </si>
+  <si>
+    <t>Nav</t>
+  </si>
+  <si>
+    <t>1. Launch Application
+2. Click links on tool bar</t>
+  </si>
+  <si>
+    <t>Checks if user can navigate throught the pages</t>
+  </si>
+  <si>
+    <t>User can navigate</t>
+  </si>
+  <si>
+    <t>User can navigate through the pages</t>
+  </si>
+  <si>
+    <t>List Pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Launch Application
+2. Click e.g Show books
+</t>
+  </si>
+  <si>
+    <t>Checks if list data is being displayed it</t>
+  </si>
+  <si>
+    <t>Data Should be displayed</t>
+  </si>
+  <si>
+    <t>Data is being displayed</t>
+  </si>
+  <si>
+    <t>Add Book</t>
+  </si>
+  <si>
+    <t>1. Launch Application
+2. Click add book
+3. Enter Test Data
+4.See if data is added</t>
+  </si>
+  <si>
+    <t>Checks if you can add a book to the database</t>
+  </si>
+  <si>
+    <t>Book should be added</t>
+  </si>
+  <si>
+    <t>Book is add to the database</t>
+  </si>
+  <si>
+    <t>Error Handling</t>
+  </si>
+  <si>
+    <t>book error</t>
+  </si>
+  <si>
+    <t>1. Launch Application
+2. Click add book
+3. Enter no Test Data</t>
+  </si>
+  <si>
+    <t>Checks if an error is displayed next to input box</t>
+  </si>
+  <si>
+    <t>error should be displayed</t>
+  </si>
+  <si>
+    <t>Error is displayed</t>
+  </si>
+  <si>
+    <t>Add customer</t>
+  </si>
+  <si>
+    <t>1. Launch Application
+2. Click add Customer
+3. Enter Test Data
+4.See if data is added</t>
+  </si>
+  <si>
+    <t>Checks if you can add a customer to the database</t>
+  </si>
+  <si>
+    <t>customer should be added</t>
+  </si>
+  <si>
+    <t>customer is add to the database</t>
+  </si>
+  <si>
+    <t>1. Launch Application
+2. Click add customer
+3. Enter no Test Data</t>
+  </si>
+  <si>
+    <t>Add Loan</t>
+  </si>
+  <si>
+    <t>1. Launch Application
+2. Click add loan
+3. Enter Test Data
+4.See if data is added</t>
+  </si>
+  <si>
+    <t>Checks if you can add a loan to the database</t>
+  </si>
+  <si>
+    <t>loan should be added</t>
+  </si>
+  <si>
+    <t>loan is add to the database</t>
+  </si>
+  <si>
+    <t>Customer error</t>
+  </si>
+  <si>
+    <t>1. Launch Application
+2. Click add loan
+3. Enter Invalid customer id and valid book ID
+4.See if error is displayed
+5.Enter valid customer id and invalid book ID
+6.See if error is displayed
+7.Enter invalid customer id and invalid book ID
+8.See if error is displayed</t>
+  </si>
+  <si>
+    <t>Checks if an appropriate Error is displayed</t>
+  </si>
+  <si>
+    <t>An error should be displayed related to the invalid data that was entered</t>
+  </si>
+  <si>
+    <t>Appropriate Error was displayed on the error page</t>
+  </si>
+  <si>
+    <t>TC.009</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Launch Application
+2. Click any of the links
+3. Enter user for the username and user for the password
+</t>
+  </si>
+  <si>
+    <t>Checks if the user can login in</t>
+  </si>
+  <si>
+    <t>User should be able to log in</t>
+  </si>
+  <si>
+    <t>User can login</t>
+  </si>
+  <si>
+    <t>TC.010</t>
+  </si>
+  <si>
+    <t>Log out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Launch Application
+2. Click any of the links
+3. Enter user for the username and user for the password
+4. Go to List Books
+5. Click Log out
+</t>
+  </si>
+  <si>
+    <t>Checks if the user can log out</t>
+  </si>
+  <si>
+    <t>User should be able to log out</t>
+  </si>
+  <si>
+    <t>User can log out</t>
   </si>
 </sst>
 </file>
@@ -948,7 +992,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1113,9 +1157,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1216,12 +1257,150 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="39">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1730,9 +1909,9 @@
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="70"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1762,11 +1941,11 @@
     <row r="6" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="72" t="s">
+      <c r="C6" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="73"/>
-      <c r="E6" s="74"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="73"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -1775,10 +1954,10 @@
       <c r="C7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="75" t="s">
+      <c r="D7" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="76"/>
+      <c r="E7" s="75"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -1787,10 +1966,10 @@
       <c r="C8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="77" t="s">
+      <c r="D8" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="78"/>
+      <c r="E8" s="77"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1815,10 +1994,10 @@
       <c r="C11" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="79" t="s">
+      <c r="D11" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="80"/>
+      <c r="E11" s="79"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1827,10 +2006,10 @@
       <c r="C12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="81" t="s">
+      <c r="D12" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="82"/>
+      <c r="E12" s="81"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1839,8 +2018,8 @@
       <c r="C13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="64"/>
-      <c r="E13" s="65"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="64"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1878,11 +2057,11 @@
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="66" t="s">
+      <c r="C18" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="67"/>
-      <c r="E18" s="68"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="67"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2149,8 +2328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2170,17 +2349,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="61"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="62" t="s">
+      <c r="A1" s="60"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="83" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="83"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
+      <c r="D1" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="82"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
       <c r="H1" s="29"/>
       <c r="I1" s="29"/>
       <c r="J1" s="29"/>
@@ -2188,16 +2367,16 @@
       <c r="L1" s="29"/>
     </row>
     <row r="2" spans="1:12" ht="134.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="84" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="F2" s="86"/>
+      <c r="A2" s="83" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="85"/>
       <c r="G2" s="31"/>
       <c r="H2" s="31"/>
       <c r="I2" s="31"/>
@@ -2216,7 +2395,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" s="54" t="s">
         <v>13</v>
@@ -2228,10 +2407,10 @@
         <v>15</v>
       </c>
       <c r="H3" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="54" t="s">
         <v>53</v>
-      </c>
-      <c r="I3" s="54" t="s">
-        <v>54</v>
       </c>
       <c r="J3" s="54" t="s">
         <v>16</v>
@@ -2243,560 +2422,600 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="60" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="59">
+    <row r="4" spans="1:12" s="59" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="58">
         <v>1</v>
       </c>
-      <c r="B4" s="57">
+      <c r="B4" s="56">
         <v>1</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="57" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="57" t="s">
+      <c r="D4" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="56" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" s="56" t="s">
-        <v>64</v>
-      </c>
-      <c r="H4" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="J4" s="57" t="s">
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+    </row>
+    <row r="5" spans="1:12" s="59" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="58">
+        <v>2</v>
+      </c>
+      <c r="B5" s="56">
+        <v>1</v>
+      </c>
+      <c r="C5" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-    </row>
-    <row r="5" spans="1:12" s="60" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="59">
-        <v>2</v>
-      </c>
-      <c r="B5" s="57">
+      <c r="D5" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="55" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="J5" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="57"/>
+      <c r="L5" s="56"/>
+    </row>
+    <row r="6" spans="1:12" s="59" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="58">
+        <v>3</v>
+      </c>
+      <c r="B6" s="56">
         <v>1</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C6" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="57" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="57" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="56" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="56" t="s">
-        <v>71</v>
-      </c>
-      <c r="I5" s="56" t="s">
-        <v>72</v>
-      </c>
-      <c r="J5" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="K5" s="58"/>
-      <c r="L5" s="57"/>
-    </row>
-    <row r="6" spans="1:12" s="60" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="59">
-        <v>3</v>
-      </c>
-      <c r="B6" s="57">
+      <c r="D6" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+    </row>
+    <row r="7" spans="1:12" s="59" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="58">
+        <v>4</v>
+      </c>
+      <c r="B7" s="56">
         <v>1</v>
       </c>
-      <c r="C6" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="57" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" s="57" t="s">
+      <c r="C7" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="I7" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="J7" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="I6" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="J6" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="K6" s="57"/>
-      <c r="L6" s="57"/>
-    </row>
-    <row r="7" spans="1:12" s="60" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="59">
-        <v>4</v>
-      </c>
-      <c r="B7" s="57">
+      <c r="K7" s="56"/>
+      <c r="L7" s="56"/>
+    </row>
+    <row r="8" spans="1:12" s="59" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="58">
+        <v>5</v>
+      </c>
+      <c r="B8" s="56">
         <v>1</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C8" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="57" t="s">
+      <c r="D8" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="56" t="s">
+      <c r="K8" s="56"/>
+      <c r="L8" s="56"/>
+    </row>
+    <row r="9" spans="1:12" s="59" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="58">
+        <v>6</v>
+      </c>
+      <c r="B9" s="56">
+        <v>1</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="H7" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="I7" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="J7" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="K7" s="57"/>
-      <c r="L7" s="57"/>
-    </row>
-    <row r="8" spans="1:12" s="60" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="59">
-        <v>5</v>
-      </c>
-      <c r="B8" s="57">
+      <c r="E9" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="J9" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+    </row>
+    <row r="10" spans="1:12" s="59" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="58">
+        <v>7</v>
+      </c>
+      <c r="B10" s="56">
         <v>1</v>
       </c>
-      <c r="C8" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="58" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" s="57" t="s">
-        <v>68</v>
-      </c>
-      <c r="F8" s="56" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="56" t="s">
-        <v>88</v>
-      </c>
-      <c r="H8" s="56" t="s">
-        <v>84</v>
-      </c>
-      <c r="I8" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="J8" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="K8" s="57"/>
-      <c r="L8" s="57"/>
-    </row>
-    <row r="9" spans="1:12" s="60" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="59">
-        <v>6</v>
-      </c>
-      <c r="B9" s="57">
+      <c r="C10" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="I10" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+    </row>
+    <row r="11" spans="1:12" s="59" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="58">
+        <v>8</v>
+      </c>
+      <c r="B11" s="56">
         <v>1</v>
       </c>
-      <c r="C9" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="58" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="57" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="H9" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="I9" s="56" t="s">
-        <v>91</v>
-      </c>
-      <c r="J9" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="K9" s="57"/>
-      <c r="L9" s="57"/>
-    </row>
-    <row r="10" spans="1:12" s="60" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="59">
-        <v>7</v>
-      </c>
-      <c r="B10" s="57">
+      <c r="C11" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="I11" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="J11" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" s="56"/>
+      <c r="L11" s="56"/>
+    </row>
+    <row r="12" spans="1:12" s="59" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="58">
+        <v>9</v>
+      </c>
+      <c r="B12" s="56">
         <v>1</v>
       </c>
-      <c r="C10" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="E10" s="57" t="s">
+      <c r="C12" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="I12" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="J12" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="G10" s="56" t="s">
-        <v>94</v>
-      </c>
-      <c r="H10" s="56" t="s">
-        <v>95</v>
-      </c>
-      <c r="I10" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="J10" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="K10" s="57"/>
-      <c r="L10" s="57"/>
-    </row>
-    <row r="11" spans="1:12" s="60" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="59">
-        <v>8</v>
-      </c>
-      <c r="B11" s="57">
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+    </row>
+    <row r="13" spans="1:12" s="59" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="58">
+        <v>10</v>
+      </c>
+      <c r="B13" s="56">
         <v>1</v>
       </c>
-      <c r="C11" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="58" t="s">
-        <v>97</v>
-      </c>
-      <c r="E11" s="57" t="s">
-        <v>68</v>
-      </c>
-      <c r="F11" s="56" t="s">
-        <v>98</v>
-      </c>
-      <c r="G11" s="56" t="s">
-        <v>99</v>
-      </c>
-      <c r="H11" s="56" t="s">
-        <v>100</v>
-      </c>
-      <c r="I11" s="56" t="s">
-        <v>101</v>
-      </c>
-      <c r="J11" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-    </row>
-    <row r="12" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="59"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-    </row>
-    <row r="13" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="59"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="57"/>
-    </row>
-    <row r="14" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="57"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="57"/>
-    </row>
-    <row r="15" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="57"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="57"/>
-    </row>
-    <row r="16" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="57"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
-    </row>
-    <row r="17" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="57"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="57"/>
-      <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
-    </row>
-    <row r="18" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="57"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-    </row>
-    <row r="19" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="57"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="57"/>
-    </row>
-    <row r="20" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="57"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="57"/>
-      <c r="L20" s="57"/>
-    </row>
-    <row r="21" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="57"/>
-      <c r="B21" s="57"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="56"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="57"/>
-    </row>
-    <row r="22" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="57"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="56"/>
-      <c r="I22" s="56"/>
-      <c r="J22" s="57"/>
-      <c r="K22" s="57"/>
-      <c r="L22" s="57"/>
-    </row>
-    <row r="23" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="57"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="57"/>
-      <c r="L23" s="57"/>
-    </row>
-    <row r="24" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="57"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="57"/>
-    </row>
-    <row r="25" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="57"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="57"/>
-      <c r="L25" s="57"/>
-    </row>
-    <row r="26" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="57"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="56"/>
-      <c r="J26" s="57"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="57"/>
-    </row>
-    <row r="27" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="57"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="57"/>
-      <c r="K27" s="57"/>
-      <c r="L27" s="57"/>
-    </row>
-    <row r="28" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="57"/>
-      <c r="B28" s="57"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="57"/>
-    </row>
-    <row r="29" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="57"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="57"/>
-      <c r="K29" s="57"/>
-      <c r="L29" s="57"/>
-    </row>
-    <row r="30" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="57"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="57"/>
-    </row>
-    <row r="31" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="57"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="57"/>
-      <c r="K31" s="57"/>
-      <c r="L31" s="57"/>
+      <c r="C13" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="56" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="56" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="I13" s="55" t="s">
+        <v>113</v>
+      </c>
+      <c r="J13" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="K13" s="56"/>
+      <c r="L13" s="56"/>
+    </row>
+    <row r="14" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="89"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="89"/>
+      <c r="K14" s="89"/>
+      <c r="L14" s="89"/>
+    </row>
+    <row r="15" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="89"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="89"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="90"/>
+      <c r="I15" s="90"/>
+      <c r="J15" s="89"/>
+      <c r="K15" s="89"/>
+      <c r="L15" s="89"/>
+    </row>
+    <row r="16" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="89"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="90"/>
+      <c r="I16" s="90"/>
+      <c r="J16" s="89"/>
+      <c r="K16" s="89"/>
+      <c r="L16" s="89"/>
+    </row>
+    <row r="17" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="89"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="89"/>
+      <c r="L17" s="89"/>
+    </row>
+    <row r="18" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="89"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="90"/>
+      <c r="I18" s="90"/>
+      <c r="J18" s="89"/>
+      <c r="K18" s="89"/>
+      <c r="L18" s="89"/>
+    </row>
+    <row r="19" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="89"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="89"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="90"/>
+      <c r="I19" s="90"/>
+      <c r="J19" s="89"/>
+      <c r="K19" s="89"/>
+      <c r="L19" s="89"/>
+    </row>
+    <row r="20" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="89"/>
+      <c r="B20" s="89"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="92"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="90"/>
+      <c r="I20" s="90"/>
+      <c r="J20" s="89"/>
+      <c r="K20" s="89"/>
+      <c r="L20" s="89"/>
+    </row>
+    <row r="21" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="89"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="89"/>
+      <c r="F21" s="91"/>
+      <c r="G21" s="90"/>
+      <c r="H21" s="90"/>
+      <c r="I21" s="90"/>
+      <c r="J21" s="89"/>
+      <c r="K21" s="89"/>
+      <c r="L21" s="89"/>
+    </row>
+    <row r="22" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="89"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="89"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="90"/>
+      <c r="H22" s="90"/>
+      <c r="I22" s="90"/>
+      <c r="J22" s="89"/>
+      <c r="K22" s="89"/>
+      <c r="L22" s="89"/>
+    </row>
+    <row r="23" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="89"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="91"/>
+      <c r="G23" s="90"/>
+      <c r="H23" s="90"/>
+      <c r="I23" s="90"/>
+      <c r="J23" s="89"/>
+      <c r="K23" s="89"/>
+      <c r="L23" s="89"/>
+    </row>
+    <row r="24" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="89"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="91"/>
+      <c r="G24" s="90"/>
+      <c r="H24" s="90"/>
+      <c r="I24" s="90"/>
+      <c r="J24" s="89"/>
+      <c r="K24" s="89"/>
+      <c r="L24" s="89"/>
+    </row>
+    <row r="25" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="89"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="91"/>
+      <c r="G25" s="90"/>
+      <c r="H25" s="90"/>
+      <c r="I25" s="90"/>
+      <c r="J25" s="89"/>
+      <c r="K25" s="89"/>
+      <c r="L25" s="89"/>
+    </row>
+    <row r="26" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="89"/>
+      <c r="B26" s="89"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="91"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="90"/>
+      <c r="I26" s="90"/>
+      <c r="J26" s="89"/>
+      <c r="K26" s="89"/>
+      <c r="L26" s="89"/>
+    </row>
+    <row r="27" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="89"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="91"/>
+      <c r="G27" s="91"/>
+      <c r="H27" s="91"/>
+      <c r="I27" s="91"/>
+      <c r="J27" s="89"/>
+      <c r="K27" s="89"/>
+      <c r="L27" s="89"/>
+    </row>
+    <row r="28" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="89"/>
+      <c r="B28" s="89"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="91"/>
+      <c r="G28" s="91"/>
+      <c r="H28" s="91"/>
+      <c r="I28" s="91"/>
+      <c r="J28" s="89"/>
+      <c r="K28" s="89"/>
+      <c r="L28" s="89"/>
+    </row>
+    <row r="29" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="89"/>
+      <c r="B29" s="89"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="89"/>
+      <c r="E29" s="89"/>
+      <c r="F29" s="91"/>
+      <c r="G29" s="91"/>
+      <c r="H29" s="91"/>
+      <c r="I29" s="91"/>
+      <c r="J29" s="89"/>
+      <c r="K29" s="89"/>
+      <c r="L29" s="89"/>
+    </row>
+    <row r="30" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="89"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="91"/>
+      <c r="G30" s="91"/>
+      <c r="H30" s="91"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="89"/>
+      <c r="K30" s="89"/>
+      <c r="L30" s="89"/>
+    </row>
+    <row r="31" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="89"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="91"/>
+      <c r="G31" s="89"/>
+      <c r="H31" s="91"/>
+      <c r="I31" s="91"/>
+      <c r="J31" s="89"/>
+      <c r="K31" s="89"/>
+      <c r="L31" s="89"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F32" s="63"/>
+      <c r="F32" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2804,70 +3023,92 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:F2"/>
   </mergeCells>
-  <conditionalFormatting sqref="J1:J6 J12:J1048576">
-    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Invalid Test">
+  <conditionalFormatting sqref="J1:J6 J14:J1048576">
+    <cfRule type="containsText" dxfId="38" priority="34" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="36" priority="36" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J11">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Invalid Test">
+      <formula>NOT(ISERROR(SEARCH("Invalid Test",J11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",J11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",J11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J10)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J11">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Invalid Test">
-      <formula>NOT(ISERROR(SEARCH("Invalid Test",J11)))</formula>
+  <conditionalFormatting sqref="J12">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Invalid Test">
+      <formula>NOT(ISERROR(SEARCH("Invalid Test",J12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",J11)))</formula>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",J12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",J11)))</formula>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",J12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Invalid Test">
+      <formula>NOT(ISERROR(SEARCH("Invalid Test",J13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",J13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",J13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2913,12 +3154,12 @@
       <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" ht="133.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="89"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="88"/>
       <c r="E2" s="33" t="s">
         <v>40</v>
       </c>
@@ -2965,13 +3206,13 @@
     <mergeCell ref="A2:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",H1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>